<commit_message>
Added Tiffany Trump speech
</commit_message>
<xml_diff>
--- a/RNC/rnc.metadata.xlsx
+++ b/RNC/rnc.metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JenniferLin/Desktop/Working/2016NCtranscripts/RNC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289E5FB0-CC04-8947-8860-0DE315FB02D3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2A1BB5-A699-7448-BAA7-4DAA036D5150}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="12800" xr2:uid="{26FD5FAB-6A1E-8249-998D-6A85A48E7CFE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="12800" activeTab="1" xr2:uid="{26FD5FAB-6A1E-8249-998D-6A85A48E7CFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Monday" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="34">
   <si>
     <t>Last</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>Monday</t>
+  </si>
+  <si>
+    <t>Tiffany</t>
+  </si>
+  <si>
+    <t>rnc.trumptiffany.txt</t>
   </si>
 </sst>
 </file>
@@ -483,7 +489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CC4E94D-E7A0-254A-BB13-F8DE8F32B892}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
@@ -531,11 +537,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02EF9062-A881-C249-A648-0C6C85EB870B}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -659,6 +665,23 @@
         <v>8</v>
       </c>
       <c r="E7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added more Monday speech
</commit_message>
<xml_diff>
--- a/RNC/rnc.metadata.xlsx
+++ b/RNC/rnc.metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JenniferLin/Desktop/Working/2016NCtranscripts/RNC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2A1BB5-A699-7448-BAA7-4DAA036D5150}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3BDAA6-EB46-8F42-94E5-524F10E5EED2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="12800" activeTab="1" xr2:uid="{26FD5FAB-6A1E-8249-998D-6A85A48E7CFE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="12800" xr2:uid="{26FD5FAB-6A1E-8249-998D-6A85A48E7CFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Monday" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="54">
   <si>
     <t>Last</t>
   </si>
@@ -136,6 +136,66 @@
   </si>
   <si>
     <t>rnc.trumptiffany.txt</t>
+  </si>
+  <si>
+    <t>Melania</t>
+  </si>
+  <si>
+    <t>Giuliani</t>
+  </si>
+  <si>
+    <t>Rudy</t>
+  </si>
+  <si>
+    <t>rnc.giuliani.txt</t>
+  </si>
+  <si>
+    <t>rnc.trumpmelania.txt</t>
+  </si>
+  <si>
+    <t>Sessions</t>
+  </si>
+  <si>
+    <t>Jeff</t>
+  </si>
+  <si>
+    <t>rnc.sessions.txt</t>
+  </si>
+  <si>
+    <t>Flynn</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>rnc.flynn.txt</t>
+  </si>
+  <si>
+    <t>Ernst</t>
+  </si>
+  <si>
+    <t>Joni</t>
+  </si>
+  <si>
+    <t>rnc.ernst.txt</t>
+  </si>
+  <si>
+    <t>Robertson</t>
+  </si>
+  <si>
+    <t>Willie</t>
+  </si>
+  <si>
+    <t>rnc.robertson.txt</t>
+  </si>
+  <si>
+    <t>Perry</t>
+  </si>
+  <si>
+    <t>Rick</t>
+  </si>
+  <si>
+    <t>rnc.perry.txt</t>
   </si>
 </sst>
 </file>
@@ -487,14 +547,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CC4E94D-E7A0-254A-BB13-F8DE8F32B892}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -527,6 +590,125 @@
         <v>31</v>
       </c>
       <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" t="s">
         <v>9</v>
       </c>
     </row>
@@ -539,7 +721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02EF9062-A881-C249-A648-0C6C85EB870B}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>

</xml_diff>

<commit_message>
Added the remaining Monday speeches from Cision
</commit_message>
<xml_diff>
--- a/RNC/rnc.metadata.xlsx
+++ b/RNC/rnc.metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JenniferLin/Desktop/Working/2016NCtranscripts/RNC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE689FE7-2526-0E4F-89FE-A4EFE4D10DA1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726C186A-B057-E143-984B-1C2E11E5F5BC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="11120" xr2:uid="{26FD5FAB-6A1E-8249-998D-6A85A48E7CFE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="12800" activeTab="1" xr2:uid="{26FD5FAB-6A1E-8249-998D-6A85A48E7CFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Monday" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="116">
   <si>
     <t>Last</t>
   </si>
@@ -307,6 +307,81 @@
   </si>
   <si>
     <t>Tampa Bay Times</t>
+  </si>
+  <si>
+    <t>Luttrell</t>
+  </si>
+  <si>
+    <t>Marcus</t>
+  </si>
+  <si>
+    <t>rnc.luttrell.txt</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Pat</t>
+  </si>
+  <si>
+    <t>rnc.smithpat.txt</t>
+  </si>
+  <si>
+    <t>Geist</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>rnc.geist.txt</t>
+  </si>
+  <si>
+    <t>Sabato</t>
+  </si>
+  <si>
+    <t>Antonio</t>
+  </si>
+  <si>
+    <t>rnc.sabato.txt</t>
+  </si>
+  <si>
+    <t>McCaul</t>
+  </si>
+  <si>
+    <t>rnc.mccaul.txt</t>
+  </si>
+  <si>
+    <t>Clarke</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>rnc.clarke.txt</t>
+  </si>
+  <si>
+    <t>Cotton</t>
+  </si>
+  <si>
+    <t>Tim</t>
+  </si>
+  <si>
+    <t>rnc.cotton.txt</t>
+  </si>
+  <si>
+    <t>Beardsley</t>
+  </si>
+  <si>
+    <t>Jason</t>
+  </si>
+  <si>
+    <t>rnc.beardsley.txt</t>
+  </si>
+  <si>
+    <t>Zinke</t>
+  </si>
+  <si>
+    <t>rnc.zinke.txt</t>
   </si>
 </sst>
 </file>
@@ -661,11 +736,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CC4E94D-E7A0-254A-BB13-F8DE8F32B892}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -854,6 +929,186 @@
         <v>84</v>
       </c>
     </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" t="s">
+        <v>102</v>
+      </c>
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" t="s">
+        <v>106</v>
+      </c>
+      <c r="C15" t="s">
+        <v>107</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>111</v>
+      </c>
+      <c r="B17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>115</v>
+      </c>
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -863,7 +1118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02EF9062-A881-C249-A648-0C6C85EB870B}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>

</xml_diff>